<commit_message>
add fasilitator qcc in rekapitulasi
</commit_message>
<xml_diff>
--- a/storage/app/public/Download/template_rekapitulasi.xlsx
+++ b/storage/app/public/Download/template_rekapitulasi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\DataKaryawan\storage\app\public\Download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A42F2B-ED57-4399-8107-39D5492D1ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740270BE-E46C-458E-8F2F-E759FCC403C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{557021F8-8DB4-43E2-A420-7FBD5893AEE4}"/>
   </bookViews>
@@ -299,7 +299,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>nik</t>
   </si>
@@ -332,6 +332,9 @@
   </si>
   <si>
     <t>OCHI_leader</t>
+  </si>
+  <si>
+    <t>fasilitator_qcc</t>
   </si>
 </sst>
 </file>
@@ -382,7 +385,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -422,8 +425,25 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -431,9 +451,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -449,11 +468,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="17">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -712,8 +757,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E65646A1-D2E3-4F8F-B01D-CFDC0FB48C80}" name="Table1" displayName="Table1" ref="A1:K50" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
-  <autoFilter ref="A1:K50" xr:uid="{E65646A1-D2E3-4F8F-B01D-CFDC0FB48C80}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E65646A1-D2E3-4F8F-B01D-CFDC0FB48C80}" name="Table1" displayName="Table1" ref="A1:L50" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+  <autoFilter ref="A1:L50" xr:uid="{E65646A1-D2E3-4F8F-B01D-CFDC0FB48C80}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -725,19 +770,21 @@
     <filterColumn colId="8" hiddenButton="1"/>
     <filterColumn colId="9" hiddenButton="1"/>
     <filterColumn colId="10" hiddenButton="1"/>
+    <filterColumn colId="11" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{5B755ABE-8F91-482F-AFF4-EB558DF8E497}" name="nik" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{84F13F03-CE3E-4C43-A19A-7C555E1B0061}" name="SD" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{21932322-04A4-4E11-9B96-6FEB44654A35}" name="S" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{92FE0440-464B-4E7B-8F2A-864DCDF58281}" name="I" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{B7795708-941C-484F-8D35-5535EC8D7517}" name="A" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{C2FE270F-1F33-4435-9886-2B681C237E0A}" name="ITD" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{E264B4C4-0D38-4BE4-A45F-D103055ED41A}" name="ICP" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{3EBA1470-B1E6-4A81-A8C7-0102654854F7}" name="TD" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{802119FE-5B09-4340-9B02-43E468E6FE7B}" name="OCHI" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{BF76FE66-F429-48DC-850A-CE901CD338A0}" name="QCC" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{D2AB371D-C3C2-4E94-B882-514D2D5787E2}" name="OCHI_leader" dataDxfId="0"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{5B755ABE-8F91-482F-AFF4-EB558DF8E497}" name="nik" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{84F13F03-CE3E-4C43-A19A-7C555E1B0061}" name="SD" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{21932322-04A4-4E11-9B96-6FEB44654A35}" name="S" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{92FE0440-464B-4E7B-8F2A-864DCDF58281}" name="I" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{B7795708-941C-484F-8D35-5535EC8D7517}" name="A" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{C2FE270F-1F33-4435-9886-2B681C237E0A}" name="ITD" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{E264B4C4-0D38-4BE4-A45F-D103055ED41A}" name="ICP" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{3EBA1470-B1E6-4A81-A8C7-0102654854F7}" name="TD" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{802119FE-5B09-4340-9B02-43E468E6FE7B}" name="OCHI" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{BF76FE66-F429-48DC-850A-CE901CD338A0}" name="QCC" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{D2AB371D-C3C2-4E94-B882-514D2D5787E2}" name="OCHI_leader" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{6778771A-B1DC-4226-A769-0D998400F7E8}" name="fasilitator_qcc" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1043,7 +1090,7 @@
   <dimension ref="A1:L50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1052,682 +1099,733 @@
     <col min="2" max="2" width="8.7265625" customWidth="1"/>
     <col min="10" max="10" width="9.7265625" customWidth="1"/>
     <col min="11" max="11" width="15.26953125" customWidth="1"/>
+    <col min="12" max="12" width="16.26953125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="1"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="1"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="6"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A21" s="6"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" s="6"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" s="6"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24" s="6"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="6"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="6"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A27" s="6"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28" s="6"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A29" s="6"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" s="6"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A31" s="6"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32" s="6"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A33" s="6"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A34" s="6"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A35" s="6"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A36" s="6"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A37" s="6"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A38" s="6"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A39" s="6"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A40" s="6"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A41" s="6"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A42" s="6"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A43" s="6"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A44" s="6"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A45" s="6"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="4"/>
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A46" s="6"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A47" s="6"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A48" s="6"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A49" s="6"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A50" s="6"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4"/>
-      <c r="K50" s="4"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" s="5"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" s="5"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" s="5"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" s="5"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A24" s="5"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A25" s="5"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A26" s="5"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A27" s="5"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A28" s="5"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A29" s="5"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A30" s="5"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A31" s="5"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A32" s="5"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A33" s="5"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A34" s="5"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A35" s="5"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A36" s="5"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A37" s="5"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A38" s="5"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A39" s="5"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A40" s="5"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A41" s="5"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A42" s="5"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A43" s="5"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A44" s="5"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A45" s="5"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A46" s="5"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A47" s="5"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A48" s="5"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A49" s="5"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A50" s="5"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3"/>
+      <c r="L50" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>